<commit_message>
Testing for Ashwin Commit
</commit_message>
<xml_diff>
--- a/Last 10 User Data.xlsx
+++ b/Last 10 User Data.xlsx
@@ -197,7 +197,7 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,22 +284,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>9862</v>
+        <v>1966</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>18</v>
@@ -311,75 +311,75 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>18</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="V2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="R2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="W2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>9863</v>
+        <v>1967</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>313</v>
+        <v>162</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0</v>
@@ -400,16 +400,16 @@
         <v>7</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>0</v>
@@ -418,13 +418,13 @@
         <v>0</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>3</v>
@@ -433,30 +433,30 @@
         <v>0</v>
       </c>
       <c r="Y3" s="0" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>9864</v>
+        <v>1968</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0</v>
@@ -465,43 +465,43 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>2</v>
@@ -510,30 +510,30 @@
         <v>0</v>
       </c>
       <c r="Y4" s="0" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>9865</v>
+        <v>1969</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>197</v>
+        <v>434</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0</v>
@@ -554,140 +554,140 @@
         <v>7</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="V5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="R5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="S5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="T5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="U5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="V5" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="W5" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y5" s="0" t="n">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>9866</v>
+        <v>1970</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>410</v>
+        <v>224</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="M6" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="N6" s="0" t="n">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Y6" s="0" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>9867</v>
+        <v>1971</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>131</v>
+        <v>353</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
@@ -699,7 +699,7 @@
         <v>95</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>1</v>
@@ -708,31 +708,31 @@
         <v>6</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="U7" s="0" t="n">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="V7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W7" s="0" t="n">
         <v>2</v>
@@ -741,30 +741,30 @@
         <v>0</v>
       </c>
       <c r="Y7" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>9868</v>
+        <v>1972</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>147</v>
+        <v>264</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
@@ -773,40 +773,40 @@
         <v>0</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="V8" s="0" t="n">
         <v>2</v>
@@ -818,48 +818,48 @@
         <v>1</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>80</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>9869</v>
+        <v>1973</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>18</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>18</v>
@@ -868,22 +868,22 @@
         <v>1</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S9" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="U9" s="0" t="n">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="V9" s="0" t="n">
         <v>5</v>
@@ -892,63 +892,63 @@
         <v>3</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="0" t="n">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9870</v>
+        <v>1974</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>234</v>
+        <v>313</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R10" s="0" t="n">
         <v>0</v>
@@ -957,45 +957,45 @@
         <v>0</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="V10" s="0" t="n">
         <v>4</v>
       </c>
       <c r="W10" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y10" s="0" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9871</v>
+        <v>1975</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0</v>
@@ -1004,46 +1004,46 @@
         <v>0</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="O11" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O11" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="P11" s="0" t="n">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S11" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="V11" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X11" s="0" t="n">
         <v>0</v>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:Y11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:Y11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>